<commit_message>
Updated Service stack results.
Let's be fair to it and send reused text reader instead of passing in to more appropriate stream API.
</commit_message>
<xml_diff>
--- a/results/result-dotnet-vs-mono.xlsx
+++ b/results/result-dotnet-vs-mono.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="7065" yWindow="840" windowWidth="15075" windowHeight="8970"/>
@@ -14,7 +14,7 @@
     <sheet name="Standard Post" sheetId="9" r:id="rId5"/>
     <sheet name="Large Book" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -99,11 +99,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,17 +379,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="hr-HR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -409,15 +399,12 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -432,7 +419,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Small Message'!$C$21:$N$21</c:f>
@@ -493,7 +479,7 @@
                   <c:v>15361.199999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28300.400000000001</c:v>
+                  <c:v>16081.999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>14168</c:v>
@@ -511,7 +497,7 @@
                   <c:v>27540.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36595.399999999994</c:v>
+                  <c:v>19410.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>41215</c:v>
@@ -537,7 +523,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Small Message'!$C$21:$N$21</c:f>
@@ -598,7 +583,7 @@
                   <c:v>36758.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37764.399999999994</c:v>
+                  <c:v>24752.400000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>14586.2</c:v>
@@ -616,7 +601,7 @@
                   <c:v>48161.000000000007</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52083.000000000015</c:v>
+                  <c:v>35843.399999999994</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>24230.200000000004</c:v>
@@ -628,42 +613,30 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="163764480"/>
-        <c:axId val="170549248"/>
+        <c:dLbls/>
+        <c:axId val="106287488"/>
+        <c:axId val="106289024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="163764480"/>
+        <c:axId val="106287488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170549248"/>
+        <c:crossAx val="106289024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170549248"/>
+        <c:axId val="106289024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -684,13 +657,10 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163764480"/>
+        <c:crossAx val="106287488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -698,15 +668,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -714,17 +682,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="hr-HR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -744,15 +702,12 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -767,7 +722,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Small Complex'!$C$21:$N$21</c:f>
@@ -828,7 +782,7 @@
                   <c:v>27599.800000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44909</c:v>
+                  <c:v>31101</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>23410.199999999997</c:v>
@@ -846,7 +800,7 @@
                   <c:v>41627.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>49885</c:v>
+                  <c:v>31722.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>50049.200000000004</c:v>
@@ -872,7 +826,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Small Complex'!$C$21:$N$21</c:f>
@@ -933,7 +886,7 @@
                   <c:v>57867.799999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48375.6</c:v>
+                  <c:v>36412.200000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>21708.600000000006</c:v>
@@ -951,7 +904,7 @@
                   <c:v>84276.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>69515.600000000006</c:v>
+                  <c:v>52770.600000000006</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>25278.399999999994</c:v>
@@ -963,42 +916,30 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="164284288"/>
-        <c:axId val="164285824"/>
+        <c:dLbls/>
+        <c:axId val="108981632"/>
+        <c:axId val="110634112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164284288"/>
+        <c:axId val="108981632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164285824"/>
+        <c:crossAx val="110634112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164285824"/>
+        <c:axId val="110634112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1019,13 +960,10 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164284288"/>
+        <c:crossAx val="108981632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1033,15 +971,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1049,17 +985,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="hr-HR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1079,15 +1005,12 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1102,7 +1025,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Small Post'!$C$21:$N$21</c:f>
@@ -1163,7 +1085,7 @@
                   <c:v>34277.800000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45947.600000000006</c:v>
+                  <c:v>31700.999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>17507.800000000003</c:v>
@@ -1181,7 +1103,7 @@
                   <c:v>107003.20000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>58285.2</c:v>
+                  <c:v>40772</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>54871.000000000007</c:v>
@@ -1204,7 +1126,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Small Post'!$C$21:$N$21</c:f>
@@ -1265,7 +1186,7 @@
                   <c:v>71904.399999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75108</c:v>
+                  <c:v>62699.600000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>30611.999999999993</c:v>
@@ -1283,7 +1204,7 @@
                   <c:v>106663.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>107222.59999999998</c:v>
+                  <c:v>87443.200000000012</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>43987.4</c:v>
@@ -1292,42 +1213,30 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="170931712"/>
-        <c:axId val="170933248"/>
+        <c:dLbls/>
+        <c:axId val="137786496"/>
+        <c:axId val="137788032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170931712"/>
+        <c:axId val="137786496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170933248"/>
+        <c:crossAx val="137788032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170933248"/>
+        <c:axId val="137788032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1348,13 +1257,10 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170931712"/>
+        <c:crossAx val="137786496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1362,15 +1268,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1378,17 +1282,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="hr-HR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1408,15 +1302,12 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1431,7 +1322,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Standard Delete'!$C$21:$N$21</c:f>
@@ -1489,7 +1379,7 @@
                   <c:v>2867</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8357.2000000000007</c:v>
+                  <c:v>6598.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>10012</c:v>
@@ -1498,7 +1388,7 @@
                   <c:v>4314.4000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9812</c:v>
+                  <c:v>7592.2000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1518,7 +1408,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Standard Delete'!$C$21:$N$21</c:f>
@@ -1576,7 +1465,7 @@
                   <c:v>6121.0000000000009</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12019.8</c:v>
+                  <c:v>10723.800000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>16452.2</c:v>
@@ -1585,48 +1474,36 @@
                   <c:v>10938.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17423.199999999997</c:v>
+                  <c:v>15312.599999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="170628224"/>
-        <c:axId val="170629760"/>
+        <c:dLbls/>
+        <c:axId val="145953536"/>
+        <c:axId val="146343040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170628224"/>
+        <c:axId val="145953536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170629760"/>
+        <c:crossAx val="146343040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170629760"/>
+        <c:axId val="146343040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1647,13 +1524,10 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170628224"/>
+        <c:crossAx val="145953536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1661,15 +1535,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1677,17 +1549,7 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="hr-HR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1707,15 +1569,12 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1730,7 +1589,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Standard Post'!$C$21:$N$21</c:f>
@@ -1788,7 +1646,7 @@
                   <c:v>62856.399999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>211564.6</c:v>
+                  <c:v>202323.19999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>416624</c:v>
@@ -1797,7 +1655,7 @@
                   <c:v>106170.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>230224.2</c:v>
+                  <c:v>212467.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1817,7 +1675,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Standard Post'!$C$21:$N$21</c:f>
@@ -1875,7 +1732,7 @@
                   <c:v>115733.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>449644.4</c:v>
+                  <c:v>472085.80000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>362586.20000000007</c:v>
@@ -1884,48 +1741,36 @@
                   <c:v>194038.40000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>576294.80000000005</c:v>
+                  <c:v>566333.80000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="170792832"/>
-        <c:axId val="170794368"/>
+        <c:dLbls/>
+        <c:axId val="155184512"/>
+        <c:axId val="155694208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170792832"/>
+        <c:axId val="155184512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170794368"/>
+        <c:crossAx val="155694208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170794368"/>
+        <c:axId val="155694208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1946,13 +1791,10 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170792832"/>
+        <c:crossAx val="155184512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1960,15 +1802,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1976,17 +1816,7 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="hr-HR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2006,15 +1836,12 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2029,7 +1856,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Large Book'!$C$21:$N$21</c:f>
@@ -2110,7 +1936,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Large Book'!$C$21:$N$21</c:f>
@@ -2177,42 +2002,30 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="171018112"/>
-        <c:axId val="171019648"/>
+        <c:dLbls/>
+        <c:axId val="157633152"/>
+        <c:axId val="158097408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171018112"/>
+        <c:axId val="157633152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171019648"/>
+        <c:crossAx val="158097408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171019648"/>
+        <c:axId val="158097408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -2233,13 +2046,10 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171018112"/>
+        <c:crossAx val="157633152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2247,15 +2057,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2498,18 +2306,18 @@
   <autoFilter ref="B21:N25"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Average"/>
-    <tableColumn id="2" name="Newtonsoft (.NET)" dataDxfId="11"/>
-    <tableColumn id="3" name="Revenj (.NET)" dataDxfId="10"/>
-    <tableColumn id="11" name="fastJSON (.NET)" dataDxfId="9"/>
-    <tableColumn id="4" name="Service Stack (.NET)" dataDxfId="8"/>
-    <tableColumn id="8" name="Jil (.NET)" dataDxfId="7"/>
-    <tableColumn id="7" name="NetJSON (.NET)" dataDxfId="6"/>
-    <tableColumn id="5" name="Newtonsoft (Mono)" dataDxfId="59"/>
-    <tableColumn id="6" name="Revenj (Mono)" dataDxfId="58"/>
-    <tableColumn id="9" name="fastJSON (Mono)" dataDxfId="57"/>
-    <tableColumn id="13" name="Service Stack (Mono)" dataDxfId="56"/>
-    <tableColumn id="12" name="Jil (Mono)" dataDxfId="55"/>
-    <tableColumn id="10" name="NetJSON (Mono)" dataDxfId="54"/>
+    <tableColumn id="2" name="Newtonsoft (.NET)" dataDxfId="59"/>
+    <tableColumn id="3" name="Revenj (.NET)" dataDxfId="58"/>
+    <tableColumn id="11" name="fastJSON (.NET)" dataDxfId="57"/>
+    <tableColumn id="4" name="Service Stack (.NET)" dataDxfId="1"/>
+    <tableColumn id="8" name="Jil (.NET)" dataDxfId="56"/>
+    <tableColumn id="7" name="NetJSON (.NET)" dataDxfId="55"/>
+    <tableColumn id="5" name="Newtonsoft (Mono)" dataDxfId="54"/>
+    <tableColumn id="6" name="Revenj (Mono)" dataDxfId="53"/>
+    <tableColumn id="9" name="fastJSON (Mono)" dataDxfId="52"/>
+    <tableColumn id="13" name="Service Stack (Mono)" dataDxfId="51"/>
+    <tableColumn id="12" name="Jil (Mono)" dataDxfId="50"/>
+    <tableColumn id="10" name="NetJSON (Mono)" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2520,18 +2328,18 @@
   <autoFilter ref="B21:N25"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Average"/>
-    <tableColumn id="2" name="Newtonsoft (.NET)" dataDxfId="5"/>
-    <tableColumn id="3" name="Revenj (.NET)" dataDxfId="4"/>
-    <tableColumn id="11" name="fastJSON (.NET)" dataDxfId="3"/>
-    <tableColumn id="4" name="Service Stack (.NET)" dataDxfId="2"/>
-    <tableColumn id="8" name="Jil (.NET)" dataDxfId="1"/>
-    <tableColumn id="7" name="NetJSON (.NET)" dataDxfId="0"/>
-    <tableColumn id="5" name="Newtonsoft (Mono)" dataDxfId="53"/>
-    <tableColumn id="6" name="Revenj (Mono)" dataDxfId="52"/>
-    <tableColumn id="9" name="fastJSON (Mono)" dataDxfId="51"/>
-    <tableColumn id="13" name="Service Stack (Mono)" dataDxfId="50"/>
-    <tableColumn id="12" name="Jil (Mono)" dataDxfId="49"/>
-    <tableColumn id="10" name="NetJSON (Mono)" dataDxfId="48"/>
+    <tableColumn id="2" name="Newtonsoft (.NET)" dataDxfId="48"/>
+    <tableColumn id="3" name="Revenj (.NET)" dataDxfId="47"/>
+    <tableColumn id="11" name="fastJSON (.NET)" dataDxfId="46"/>
+    <tableColumn id="4" name="Service Stack (.NET)" dataDxfId="0"/>
+    <tableColumn id="8" name="Jil (.NET)" dataDxfId="45"/>
+    <tableColumn id="7" name="NetJSON (.NET)" dataDxfId="44"/>
+    <tableColumn id="5" name="Newtonsoft (Mono)" dataDxfId="43"/>
+    <tableColumn id="6" name="Revenj (Mono)" dataDxfId="42"/>
+    <tableColumn id="9" name="fastJSON (Mono)" dataDxfId="41"/>
+    <tableColumn id="13" name="Service Stack (Mono)" dataDxfId="40"/>
+    <tableColumn id="12" name="Jil (Mono)" dataDxfId="39"/>
+    <tableColumn id="10" name="NetJSON (Mono)" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2542,18 +2350,18 @@
   <autoFilter ref="B21:N25"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Average"/>
-    <tableColumn id="2" name="Newtonsoft (.NET)" dataDxfId="47"/>
-    <tableColumn id="3" name="Revenj (.NET)" dataDxfId="46"/>
-    <tableColumn id="11" name="fastJSON (.NET)" dataDxfId="45"/>
-    <tableColumn id="4" name="Service Stack (.NET)" dataDxfId="44"/>
-    <tableColumn id="8" name="Jil (.NET)" dataDxfId="43"/>
-    <tableColumn id="7" name="NetJSON (.NET)" dataDxfId="42"/>
-    <tableColumn id="5" name="Newtonsoft (Mono)" dataDxfId="41"/>
-    <tableColumn id="6" name="Revenj (Mono)" dataDxfId="40"/>
-    <tableColumn id="9" name="fastJSON (Mono)" dataDxfId="39"/>
-    <tableColumn id="13" name="Service Stack (Mono)" dataDxfId="38"/>
-    <tableColumn id="12" name="Jil (Mono)" dataDxfId="37"/>
-    <tableColumn id="10" name="NetJSON (Mono)" dataDxfId="36"/>
+    <tableColumn id="2" name="Newtonsoft (.NET)" dataDxfId="37"/>
+    <tableColumn id="3" name="Revenj (.NET)" dataDxfId="36"/>
+    <tableColumn id="11" name="fastJSON (.NET)" dataDxfId="35"/>
+    <tableColumn id="4" name="Service Stack (.NET)" dataDxfId="34"/>
+    <tableColumn id="8" name="Jil (.NET)" dataDxfId="33"/>
+    <tableColumn id="7" name="NetJSON (.NET)" dataDxfId="32"/>
+    <tableColumn id="5" name="Newtonsoft (Mono)" dataDxfId="31"/>
+    <tableColumn id="6" name="Revenj (Mono)" dataDxfId="30"/>
+    <tableColumn id="9" name="fastJSON (Mono)" dataDxfId="29"/>
+    <tableColumn id="13" name="Service Stack (Mono)" dataDxfId="28"/>
+    <tableColumn id="12" name="Jil (Mono)" dataDxfId="27"/>
+    <tableColumn id="10" name="NetJSON (Mono)" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2564,18 +2372,18 @@
   <autoFilter ref="B21:N25"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Average"/>
-    <tableColumn id="2" name="Newtonsoft (.NET)" dataDxfId="35"/>
-    <tableColumn id="3" name="Revenj (.NET)" dataDxfId="34"/>
-    <tableColumn id="11" name="fastJSON (.NET)" dataDxfId="33"/>
-    <tableColumn id="4" name="Service Stack (.NET)" dataDxfId="32"/>
-    <tableColumn id="8" name="Jil (.NET)" dataDxfId="31"/>
-    <tableColumn id="7" name="NetJSON (.NET)" dataDxfId="30"/>
-    <tableColumn id="5" name="Newtonsoft (Mono)" dataDxfId="29"/>
-    <tableColumn id="6" name="Revenj (Mono)" dataDxfId="28"/>
-    <tableColumn id="9" name="fastJSON (Mono)" dataDxfId="27"/>
-    <tableColumn id="13" name="Service Stack (Mono)" dataDxfId="26"/>
-    <tableColumn id="12" name="Jil (Mono)" dataDxfId="25"/>
-    <tableColumn id="10" name="NetJSON (Mono)" dataDxfId="24"/>
+    <tableColumn id="2" name="Newtonsoft (.NET)" dataDxfId="25"/>
+    <tableColumn id="3" name="Revenj (.NET)" dataDxfId="24"/>
+    <tableColumn id="11" name="fastJSON (.NET)" dataDxfId="23"/>
+    <tableColumn id="4" name="Service Stack (.NET)" dataDxfId="22"/>
+    <tableColumn id="8" name="Jil (.NET)" dataDxfId="21"/>
+    <tableColumn id="7" name="NetJSON (.NET)" dataDxfId="20"/>
+    <tableColumn id="5" name="Newtonsoft (Mono)" dataDxfId="19"/>
+    <tableColumn id="6" name="Revenj (Mono)" dataDxfId="18"/>
+    <tableColumn id="9" name="fastJSON (Mono)" dataDxfId="17"/>
+    <tableColumn id="13" name="Service Stack (Mono)" dataDxfId="16"/>
+    <tableColumn id="12" name="Jil (Mono)" dataDxfId="15"/>
+    <tableColumn id="10" name="NetJSON (Mono)" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2586,18 +2394,18 @@
   <autoFilter ref="B21:N25"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Average"/>
-    <tableColumn id="2" name="Newtonsoft (.NET) - DSL model" dataDxfId="23"/>
-    <tableColumn id="3" name="Revenj (.NET)" dataDxfId="22"/>
-    <tableColumn id="11" name="fastJSON (.NET)" dataDxfId="21"/>
-    <tableColumn id="4" name="Service Stack (.NET)" dataDxfId="20"/>
-    <tableColumn id="8" name="Jil (.NET)" dataDxfId="19"/>
-    <tableColumn id="7" name="NetJSON (.NET)" dataDxfId="18"/>
-    <tableColumn id="5" name="Newtonsoft (Mono) - DSL model" dataDxfId="17"/>
-    <tableColumn id="6" name="Revenj (Mono)" dataDxfId="16"/>
-    <tableColumn id="9" name="fastJSON (Mono)" dataDxfId="15"/>
-    <tableColumn id="13" name="Service Stack (Mono)" dataDxfId="14"/>
-    <tableColumn id="12" name="Jil (Mono)" dataDxfId="13"/>
-    <tableColumn id="10" name="NetJSON (Mono)" dataDxfId="12"/>
+    <tableColumn id="2" name="Newtonsoft (.NET) - DSL model" dataDxfId="13"/>
+    <tableColumn id="3" name="Revenj (.NET)" dataDxfId="12"/>
+    <tableColumn id="11" name="fastJSON (.NET)" dataDxfId="11"/>
+    <tableColumn id="4" name="Service Stack (.NET)" dataDxfId="10"/>
+    <tableColumn id="8" name="Jil (.NET)" dataDxfId="9"/>
+    <tableColumn id="7" name="NetJSON (.NET)" dataDxfId="8"/>
+    <tableColumn id="5" name="Newtonsoft (Mono) - DSL model" dataDxfId="7"/>
+    <tableColumn id="6" name="Revenj (Mono)" dataDxfId="6"/>
+    <tableColumn id="9" name="fastJSON (Mono)" dataDxfId="5"/>
+    <tableColumn id="13" name="Service Stack (Mono)" dataDxfId="4"/>
+    <tableColumn id="12" name="Jil (Mono)" dataDxfId="3"/>
+    <tableColumn id="10" name="NetJSON (Mono)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2678,7 +2486,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2713,7 +2520,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2889,14 +2695,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
@@ -2921,12 +2727,12 @@
     <col min="24" max="24" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -2967,7 +2773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17">
       <c r="B22" t="s">
         <v>2</v>
       </c>
@@ -2999,7 +2805,7 @@
         <v>9097</v>
       </c>
       <c r="L22" s="1">
-        <v>8973.2000000000007</v>
+        <v>9608.7999999999993</v>
       </c>
       <c r="M22" s="1">
         <v>9275.4</v>
@@ -3011,7 +2817,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -3025,7 +2831,7 @@
         <v>15361.199999999999</v>
       </c>
       <c r="F23" s="1">
-        <v>28300.400000000001</v>
+        <v>16081.999999999998</v>
       </c>
       <c r="G23" s="1">
         <v>14168</v>
@@ -3043,7 +2849,7 @@
         <v>27540.6</v>
       </c>
       <c r="L23" s="1">
-        <v>36595.399999999994</v>
+        <v>19410.8</v>
       </c>
       <c r="M23" s="1">
         <v>41215</v>
@@ -3055,7 +2861,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -3069,7 +2875,7 @@
         <v>36758.6</v>
       </c>
       <c r="F24" s="1">
-        <v>37764.399999999994</v>
+        <v>24752.400000000001</v>
       </c>
       <c r="G24" s="1">
         <v>14586.2</v>
@@ -3087,7 +2893,7 @@
         <v>48161.000000000007</v>
       </c>
       <c r="L24" s="1">
-        <v>52083.000000000015</v>
+        <v>35843.399999999994</v>
       </c>
       <c r="M24" s="1">
         <v>24230.200000000004</v>
@@ -3099,7 +2905,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17">
       <c r="B25" t="s">
         <v>5</v>
       </c>
@@ -3113,7 +2919,7 @@
         <v>56682.2</v>
       </c>
       <c r="F25" s="1">
-        <v>70744.399999999994</v>
+        <v>45514</v>
       </c>
       <c r="G25" s="1">
         <v>33505.4</v>
@@ -3131,7 +2937,7 @@
         <v>84798.6</v>
       </c>
       <c r="L25" s="1">
-        <v>97651.6</v>
+        <v>64863</v>
       </c>
       <c r="M25" s="1">
         <v>74720.600000000006</v>
@@ -3143,10 +2949,10 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17">
       <c r="D27" s="1"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -3163,7 +2969,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -3180,20 +2986,20 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17">
       <c r="B32" s="2"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2">
       <c r="B40" s="2"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2">
       <c r="B48" s="2"/>
     </row>
   </sheetData>
@@ -3207,14 +3013,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
@@ -3239,12 +3045,12 @@
     <col min="24" max="24" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -3285,7 +3091,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17">
       <c r="B22" t="s">
         <v>2</v>
       </c>
@@ -3317,7 +3123,7 @@
         <v>6758.6</v>
       </c>
       <c r="L22" s="1">
-        <v>6841.4</v>
+        <v>6694.4</v>
       </c>
       <c r="M22" s="1">
         <v>6987.6</v>
@@ -3329,7 +3135,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -3343,7 +3149,7 @@
         <v>27599.800000000003</v>
       </c>
       <c r="F23" s="1">
-        <v>44909</v>
+        <v>31101</v>
       </c>
       <c r="G23" s="1">
         <v>23410.199999999997</v>
@@ -3361,7 +3167,7 @@
         <v>41627.4</v>
       </c>
       <c r="L23" s="1">
-        <v>49885</v>
+        <v>31722.6</v>
       </c>
       <c r="M23" s="1">
         <v>50049.200000000004</v>
@@ -3373,7 +3179,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -3387,7 +3193,7 @@
         <v>57867.799999999996</v>
       </c>
       <c r="F24" s="1">
-        <v>48375.6</v>
+        <v>36412.200000000004</v>
       </c>
       <c r="G24" s="1">
         <v>21708.600000000006</v>
@@ -3405,7 +3211,7 @@
         <v>84276.4</v>
       </c>
       <c r="L24" s="1">
-        <v>69515.600000000006</v>
+        <v>52770.600000000006</v>
       </c>
       <c r="M24" s="1">
         <v>25278.399999999994</v>
@@ -3417,7 +3223,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17">
       <c r="B25" t="s">
         <v>5</v>
       </c>
@@ -3431,7 +3237,7 @@
         <v>90832.2</v>
       </c>
       <c r="F25" s="1">
-        <v>98325</v>
+        <v>72553.600000000006</v>
       </c>
       <c r="G25" s="1">
         <v>50176.4</v>
@@ -3449,7 +3255,7 @@
         <v>132662.39999999999</v>
       </c>
       <c r="L25" s="1">
-        <v>126242</v>
+        <v>91187.6</v>
       </c>
       <c r="M25" s="1">
         <v>82315.199999999997</v>
@@ -3461,10 +3267,10 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17">
       <c r="D27" s="1"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -3481,7 +3287,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -3498,20 +3304,20 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17">
       <c r="B32" s="2"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2">
       <c r="B40" s="2"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2">
       <c r="B48" s="2"/>
     </row>
   </sheetData>
@@ -3525,14 +3331,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
@@ -3557,12 +3363,12 @@
     <col min="24" max="24" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -3603,7 +3409,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17">
       <c r="B22" t="s">
         <v>2</v>
       </c>
@@ -3635,7 +3441,7 @@
         <v>33482.400000000001</v>
       </c>
       <c r="L22" s="1">
-        <v>33820</v>
+        <v>33514</v>
       </c>
       <c r="M22" s="1">
         <v>33577.599999999999</v>
@@ -3647,7 +3453,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -3661,7 +3467,7 @@
         <v>34277.800000000003</v>
       </c>
       <c r="F23" s="1">
-        <v>45947.600000000006</v>
+        <v>31700.999999999996</v>
       </c>
       <c r="G23" s="1">
         <v>17507.800000000003</v>
@@ -3679,7 +3485,7 @@
         <v>107003.20000000001</v>
       </c>
       <c r="L23" s="1">
-        <v>58285.2</v>
+        <v>40772</v>
       </c>
       <c r="M23" s="1">
         <v>54871.000000000007</v>
@@ -3689,7 +3495,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -3703,7 +3509,7 @@
         <v>71904.399999999994</v>
       </c>
       <c r="F24" s="1">
-        <v>75108</v>
+        <v>62699.600000000006</v>
       </c>
       <c r="G24" s="1">
         <v>30611.999999999993</v>
@@ -3721,7 +3527,7 @@
         <v>106663.6</v>
       </c>
       <c r="L24" s="1">
-        <v>107222.59999999998</v>
+        <v>87443.200000000012</v>
       </c>
       <c r="M24" s="1">
         <v>43987.4</v>
@@ -3731,7 +3537,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17">
       <c r="B25" t="s">
         <v>5</v>
       </c>
@@ -3745,7 +3551,7 @@
         <v>114139.2</v>
       </c>
       <c r="F25" s="1">
-        <v>128876.8</v>
+        <v>102221.8</v>
       </c>
       <c r="G25" s="1">
         <v>55961.2</v>
@@ -3763,7 +3569,7 @@
         <v>247149.2</v>
       </c>
       <c r="L25" s="1">
-        <v>199327.8</v>
+        <v>161729.20000000001</v>
       </c>
       <c r="M25" s="1">
         <v>132436</v>
@@ -3773,10 +3579,10 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17">
       <c r="D27" s="1"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -3793,7 +3599,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -3810,20 +3616,20 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17">
       <c r="B32" s="2"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2">
       <c r="B40" s="2"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2">
       <c r="B48" s="2"/>
     </row>
   </sheetData>
@@ -3837,14 +3643,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
@@ -3869,12 +3675,12 @@
     <col min="24" max="24" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -3915,7 +3721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17">
       <c r="B22" t="s">
         <v>2</v>
       </c>
@@ -3939,7 +3745,7 @@
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1">
-        <v>1554.4</v>
+        <v>1565</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -3947,7 +3753,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -3959,7 +3765,7 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
-        <v>8357.2000000000007</v>
+        <v>6598.4</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -3971,7 +3777,7 @@
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1">
-        <v>9812</v>
+        <v>7592.2000000000007</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -3979,7 +3785,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -3991,7 +3797,7 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1">
-        <v>12019.8</v>
+        <v>10723.800000000001</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -4003,7 +3809,7 @@
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1">
-        <v>17423.199999999997</v>
+        <v>15312.599999999999</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -4011,7 +3817,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17">
       <c r="B25" t="s">
         <v>5</v>
       </c>
@@ -4023,7 +3829,7 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1">
-        <v>22670</v>
+        <v>19615.2</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -4035,7 +3841,7 @@
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1">
-        <v>28789.599999999999</v>
+        <v>24469.8</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -4043,7 +3849,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -4060,7 +3866,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -4077,20 +3883,20 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17">
       <c r="B31" s="2"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2">
       <c r="B39" s="2"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2">
       <c r="B47" s="2"/>
     </row>
   </sheetData>
@@ -4104,14 +3910,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
@@ -4136,12 +3942,12 @@
     <col min="24" max="24" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -4182,7 +3988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17">
       <c r="B22" t="s">
         <v>2</v>
       </c>
@@ -4206,7 +4012,7 @@
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1">
-        <v>136307.79999999999</v>
+        <v>139824.20000000001</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -4214,7 +4020,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -4226,7 +4032,7 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
-        <v>211564.6</v>
+        <v>202323.19999999998</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -4238,7 +4044,7 @@
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1">
-        <v>230224.2</v>
+        <v>212467.8</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -4246,7 +4052,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -4258,7 +4064,7 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1">
-        <v>449644.4</v>
+        <v>472085.80000000005</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -4270,7 +4076,7 @@
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1">
-        <v>576294.80000000005</v>
+        <v>566333.80000000005</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -4278,7 +4084,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17">
       <c r="B25" t="s">
         <v>5</v>
       </c>
@@ -4290,7 +4096,7 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1">
-        <v>748054.6</v>
+        <v>761254.6</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -4302,7 +4108,7 @@
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1">
-        <v>942826.8</v>
+        <v>918625.8</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -4310,7 +4116,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -4327,7 +4133,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -4344,20 +4150,20 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17">
       <c r="B31" s="2"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2">
       <c r="B39" s="2"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2">
       <c r="B47" s="2"/>
     </row>
   </sheetData>
@@ -4371,14 +4177,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
@@ -4403,12 +4209,12 @@
     <col min="24" max="24" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -4449,7 +4255,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17">
       <c r="B22" t="s">
         <v>2</v>
       </c>
@@ -4477,7 +4283,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -4505,7 +4311,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -4533,7 +4339,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17">
       <c r="B25" t="s">
         <v>5</v>
       </c>
@@ -4561,7 +4367,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -4578,7 +4384,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -4595,20 +4401,20 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17">
       <c r="B32" s="2"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2">
       <c r="B40" s="2"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2">
       <c r="B48" s="2"/>
     </row>
   </sheetData>

</xml_diff>